<commit_message>
updated search assets and main script and template
</commit_message>
<xml_diff>
--- a/retail/KPIS Dashboards mapping Retail 2.0.xlsx
+++ b/retail/KPIS Dashboards mapping Retail 2.0.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorgft3817606-my.sharepoint.com/personal/kashif_mohammed_salespointinc_com/Documents/Projects/Data and AI Dream Demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDAEC0E1-3CE0-4047-955F-661B9856E05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{27224BC1-A293-4DB4-A24D-603225029E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2C026CFF-B50D-4FA4-9AD2-ED7378D91A7A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{2C026CFF-B50D-4FA4-9AD2-ED7378D91A7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$56</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="166">
   <si>
     <t>KPI</t>
   </si>
@@ -452,13 +452,94 @@
   </si>
   <si>
     <t>Pillar 4 Dec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page 5 </t>
+  </si>
+  <si>
+    <t>Dashboard Images</t>
+  </si>
+  <si>
+    <t>Chiclet- Number of Visitors</t>
+  </si>
+  <si>
+    <t>Chiclet- Checkout Time and Store Temperature</t>
+  </si>
+  <si>
+    <t>Chiclet- Aisle Dwell Time and Customer Satisfaction</t>
+  </si>
+  <si>
+    <t>Chiclet- TopLeft Corner</t>
+  </si>
+  <si>
+    <t>Page 6</t>
+  </si>
+  <si>
+    <t>Chiclet- KPI</t>
+  </si>
+  <si>
+    <t>Chiclet- Deep Dive</t>
+  </si>
+  <si>
+    <t>REtail 270821</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEO Dashboard - All Dashboards </t>
+  </si>
+  <si>
+    <t>Chiclet- Campaign Analytics</t>
+  </si>
+  <si>
+    <t>Chiclet- Realtime Social Media and Video Analytics</t>
+  </si>
+  <si>
+    <t>Chiclet- Realtime location Analytics</t>
+  </si>
+  <si>
+    <t>Chiclet- Predictive and Prescriptive Analytics</t>
+  </si>
+  <si>
+    <t>Chiclet- Income and Profitability Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chiclet- Operating Expense Mangement </t>
+  </si>
+  <si>
+    <t>Chiclet- Financial Planning and Analysis</t>
+  </si>
+  <si>
+    <t>Chiclet- Risk and Complaince Management</t>
+  </si>
+  <si>
+    <t>Chiclet- ESG Sentiment Analytics</t>
+  </si>
+  <si>
+    <t>Chiclet- Competetive Esg Metrics</t>
+  </si>
+  <si>
+    <t>Chiclet- Esg Portfolio Analytics</t>
+  </si>
+  <si>
+    <t>ESG</t>
+  </si>
+  <si>
+    <t>Chiclet- Internal Customer Alignment</t>
+  </si>
+  <si>
+    <t>Chiclet- Market Perception</t>
+  </si>
+  <si>
+    <t>Chiclet- Customer Retention and Growth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page 4 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -468,6 +549,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -499,10 +587,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,7 +615,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -817,18 +911,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E18BD886-62ED-448C-B156-45B2284206D7}">
-  <dimension ref="A1:E192"/>
+  <dimension ref="A1:E224"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E117" sqref="E117:E119"/>
+      <selection activeCell="G207" sqref="G207"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="47.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -850,121 +944,112 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>149</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>150</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>149</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>151</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="E3" t="s">
-        <v>113</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>149</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>152</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="E4" t="s">
-        <v>113</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>149</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>153</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="E5" t="s">
-        <v>113</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>144</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E6" t="s">
-        <v>113</v>
+        <v>140</v>
+      </c>
+      <c r="E6" s="3">
+        <v>44441</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
+        <v>149</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>146</v>
       </c>
       <c r="D7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E7" t="s">
-        <v>113</v>
+        <v>140</v>
+      </c>
+      <c r="E7" s="3">
+        <v>44441</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>147</v>
       </c>
       <c r="D8" t="s">
-        <v>115</v>
+        <v>140</v>
       </c>
       <c r="E8" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -972,16 +1057,16 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E9" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -989,16 +1074,16 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E10" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1006,16 +1091,16 @@
         <v>5</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E11" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1023,16 +1108,16 @@
         <v>5</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
         <v>112</v>
       </c>
       <c r="E12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1040,16 +1125,16 @@
         <v>5</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>117</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>123</v>
+        <v>112</v>
+      </c>
+      <c r="E13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1057,16 +1142,16 @@
         <v>5</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E14" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1074,16 +1159,16 @@
         <v>5</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E15" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1091,16 +1176,16 @@
         <v>5</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E16" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1108,16 +1193,16 @@
         <v>5</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E17" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1125,16 +1210,16 @@
         <v>5</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E18" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1142,16 +1227,16 @@
         <v>5</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E19" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1159,16 +1244,16 @@
         <v>5</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>112</v>
-      </c>
-      <c r="E20" t="s">
-        <v>124</v>
+        <v>117</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1176,16 +1261,16 @@
         <v>5</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="E21" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1193,16 +1278,16 @@
         <v>5</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="E22" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1210,16 +1295,16 @@
         <v>5</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E23" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1227,16 +1312,16 @@
         <v>5</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E24" t="s">
-        <v>68</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1244,135 +1329,135 @@
         <v>5</v>
       </c>
       <c r="B25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D25" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E25" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D26" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E26" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D27" t="s">
         <v>112</v>
       </c>
       <c r="E27" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D28" t="s">
         <v>112</v>
       </c>
       <c r="E28" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D29" t="s">
         <v>112</v>
       </c>
       <c r="E29" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D30" t="s">
         <v>112</v>
       </c>
       <c r="E30" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D31" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="E31" t="s">
-        <v>114</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D32" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="E32" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1380,16 +1465,16 @@
         <v>28</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E33" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1397,16 +1482,16 @@
         <v>28</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E34" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1414,16 +1499,16 @@
         <v>28</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E35" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1431,16 +1516,16 @@
         <v>28</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D36" t="s">
         <v>112</v>
       </c>
       <c r="E36" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1448,13 +1533,16 @@
         <v>28</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>117</v>
+        <v>112</v>
+      </c>
+      <c r="E37" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1462,13 +1550,16 @@
         <v>28</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D38" t="s">
-        <v>118</v>
+        <v>112</v>
+      </c>
+      <c r="E38" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1476,13 +1567,16 @@
         <v>28</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D39" t="s">
-        <v>118</v>
+        <v>115</v>
+      </c>
+      <c r="E39" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1490,16 +1584,16 @@
         <v>28</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D40" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E40" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1507,16 +1601,16 @@
         <v>28</v>
       </c>
       <c r="B41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D41" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E41" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1524,16 +1618,16 @@
         <v>28</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D42" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E42" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1541,16 +1635,16 @@
         <v>28</v>
       </c>
       <c r="B43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D43" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E43" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1558,16 +1652,13 @@
         <v>28</v>
       </c>
       <c r="B44">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D44" t="s">
-        <v>112</v>
-      </c>
-      <c r="E44" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1575,16 +1666,13 @@
         <v>28</v>
       </c>
       <c r="B45">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D45" t="s">
-        <v>112</v>
-      </c>
-      <c r="E45" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1592,16 +1680,13 @@
         <v>28</v>
       </c>
       <c r="B46">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D46" t="s">
-        <v>112</v>
-      </c>
-      <c r="E46" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1609,16 +1694,16 @@
         <v>28</v>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D47" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E47" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1626,16 +1711,16 @@
         <v>28</v>
       </c>
       <c r="B48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D48" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E48" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1643,135 +1728,135 @@
         <v>28</v>
       </c>
       <c r="B49">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D49" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E49" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D50" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E50" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D51" t="s">
         <v>112</v>
       </c>
       <c r="E51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D52" t="s">
         <v>112</v>
       </c>
       <c r="E52" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D53" t="s">
         <v>112</v>
       </c>
       <c r="E53" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D54" t="s">
         <v>112</v>
       </c>
       <c r="E54" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C55" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D55" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="E55" t="s">
-        <v>130</v>
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B56">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D56" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="E56" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -1779,16 +1864,16 @@
         <v>29</v>
       </c>
       <c r="B57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D57" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E57" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1796,16 +1881,16 @@
         <v>29</v>
       </c>
       <c r="B58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D58" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E58" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -1813,16 +1898,16 @@
         <v>29</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D59" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E59" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -1830,16 +1915,16 @@
         <v>29</v>
       </c>
       <c r="B60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D60" t="s">
         <v>112</v>
       </c>
       <c r="E60" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -1847,13 +1932,16 @@
         <v>29</v>
       </c>
       <c r="B61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D61" t="s">
-        <v>117</v>
+        <v>112</v>
+      </c>
+      <c r="E61" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -1861,13 +1949,16 @@
         <v>29</v>
       </c>
       <c r="B62">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D62" t="s">
-        <v>118</v>
+        <v>112</v>
+      </c>
+      <c r="E62" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -1875,13 +1966,16 @@
         <v>29</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C63" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D63" t="s">
-        <v>118</v>
+        <v>115</v>
+      </c>
+      <c r="E63" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -1889,16 +1983,16 @@
         <v>29</v>
       </c>
       <c r="B64">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D64" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E64" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -1906,16 +2000,16 @@
         <v>29</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C65" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D65" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E65" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -1923,16 +2017,16 @@
         <v>29</v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C66" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D66" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E66" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -1940,16 +2034,16 @@
         <v>29</v>
       </c>
       <c r="B67">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C67" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D67" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E67" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -1957,16 +2051,13 @@
         <v>29</v>
       </c>
       <c r="B68">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C68" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D68" t="s">
-        <v>112</v>
-      </c>
-      <c r="E68" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -1974,16 +2065,13 @@
         <v>29</v>
       </c>
       <c r="B69">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C69" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D69" t="s">
-        <v>112</v>
-      </c>
-      <c r="E69" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -1991,16 +2079,13 @@
         <v>29</v>
       </c>
       <c r="B70">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D70" t="s">
-        <v>112</v>
-      </c>
-      <c r="E70" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -2008,16 +2093,16 @@
         <v>29</v>
       </c>
       <c r="B71">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C71" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D71" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E71" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -2025,16 +2110,16 @@
         <v>29</v>
       </c>
       <c r="B72">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D72" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E72" t="s">
-        <v>68</v>
+        <v>128</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -2042,135 +2127,135 @@
         <v>29</v>
       </c>
       <c r="B73">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D73" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E73" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B74">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D74" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E74" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B75">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C75" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D75" t="s">
         <v>112</v>
       </c>
       <c r="E75" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B76">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C76" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D76" t="s">
         <v>112</v>
       </c>
       <c r="E76" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B77">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C77" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D77" t="s">
         <v>112</v>
       </c>
       <c r="E77" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B78">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C78" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D78" t="s">
         <v>112</v>
       </c>
       <c r="E78" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B79">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C79" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D79" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="E79" t="s">
-        <v>133</v>
+        <v>68</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B80">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C80" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D80" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="E80" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -2178,16 +2263,16 @@
         <v>30</v>
       </c>
       <c r="B81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D81" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E81" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -2195,16 +2280,16 @@
         <v>30</v>
       </c>
       <c r="B82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D82" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E82" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -2212,16 +2297,16 @@
         <v>30</v>
       </c>
       <c r="B83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D83" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E83" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -2229,16 +2314,16 @@
         <v>30</v>
       </c>
       <c r="B84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D84" t="s">
         <v>112</v>
       </c>
       <c r="E84" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -2246,13 +2331,16 @@
         <v>30</v>
       </c>
       <c r="B85">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C85" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D85" t="s">
-        <v>117</v>
+        <v>112</v>
+      </c>
+      <c r="E85" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -2260,13 +2348,16 @@
         <v>30</v>
       </c>
       <c r="B86">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C86" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D86" t="s">
-        <v>118</v>
+        <v>112</v>
+      </c>
+      <c r="E86" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -2274,13 +2365,16 @@
         <v>30</v>
       </c>
       <c r="B87">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C87" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D87" t="s">
-        <v>118</v>
+        <v>115</v>
+      </c>
+      <c r="E87" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
@@ -2288,16 +2382,16 @@
         <v>30</v>
       </c>
       <c r="B88">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C88" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D88" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E88" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -2305,16 +2399,16 @@
         <v>30</v>
       </c>
       <c r="B89">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C89" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D89" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E89" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
@@ -2322,16 +2416,16 @@
         <v>30</v>
       </c>
       <c r="B90">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C90" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D90" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E90" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
@@ -2339,16 +2433,16 @@
         <v>30</v>
       </c>
       <c r="B91">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C91" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D91" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E91" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
@@ -2356,16 +2450,13 @@
         <v>30</v>
       </c>
       <c r="B92">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C92" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D92" t="s">
-        <v>112</v>
-      </c>
-      <c r="E92" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
@@ -2373,16 +2464,13 @@
         <v>30</v>
       </c>
       <c r="B93">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C93" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D93" t="s">
-        <v>112</v>
-      </c>
-      <c r="E93" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
@@ -2390,16 +2478,13 @@
         <v>30</v>
       </c>
       <c r="B94">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C94" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D94" t="s">
-        <v>112</v>
-      </c>
-      <c r="E94" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
@@ -2407,16 +2492,16 @@
         <v>30</v>
       </c>
       <c r="B95">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C95" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D95" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E95" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
@@ -2424,16 +2509,16 @@
         <v>30</v>
       </c>
       <c r="B96">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C96" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D96" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E96" t="s">
-        <v>68</v>
+        <v>131</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
@@ -2441,135 +2526,135 @@
         <v>30</v>
       </c>
       <c r="B97">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C97" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D97" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E97" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B98">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C98" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D98" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E98" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B99">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C99" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D99" t="s">
         <v>112</v>
       </c>
       <c r="E99" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B100">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C100" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D100" t="s">
         <v>112</v>
       </c>
       <c r="E100" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B101">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C101" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D101" t="s">
         <v>112</v>
       </c>
       <c r="E101" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B102">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C102" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D102" t="s">
         <v>112</v>
       </c>
       <c r="E102" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B103">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C103" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D103" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="E103" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B104">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C104" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D104" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="E104" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
@@ -2577,16 +2662,16 @@
         <v>31</v>
       </c>
       <c r="B105">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C105" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D105" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E105" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
@@ -2594,16 +2679,16 @@
         <v>31</v>
       </c>
       <c r="B106">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C106" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D106" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E106" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
@@ -2611,16 +2696,16 @@
         <v>31</v>
       </c>
       <c r="B107">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C107" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D107" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E107" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -2628,16 +2713,16 @@
         <v>31</v>
       </c>
       <c r="B108">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C108" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D108" t="s">
         <v>112</v>
       </c>
       <c r="E108" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
@@ -2645,13 +2730,16 @@
         <v>31</v>
       </c>
       <c r="B109">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C109" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D109" t="s">
-        <v>117</v>
+        <v>112</v>
+      </c>
+      <c r="E109" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
@@ -2659,13 +2747,16 @@
         <v>31</v>
       </c>
       <c r="B110">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C110" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D110" t="s">
-        <v>118</v>
+        <v>112</v>
+      </c>
+      <c r="E110" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
@@ -2673,13 +2764,16 @@
         <v>31</v>
       </c>
       <c r="B111">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C111" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D111" t="s">
-        <v>118</v>
+        <v>115</v>
+      </c>
+      <c r="E111" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
@@ -2687,16 +2781,16 @@
         <v>31</v>
       </c>
       <c r="B112">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C112" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D112" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E112" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
@@ -2704,16 +2798,16 @@
         <v>31</v>
       </c>
       <c r="B113">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C113" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D113" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E113" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
@@ -2721,16 +2815,16 @@
         <v>31</v>
       </c>
       <c r="B114">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C114" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D114" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E114" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -2738,16 +2832,16 @@
         <v>31</v>
       </c>
       <c r="B115">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C115" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D115" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E115" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
@@ -2755,16 +2849,13 @@
         <v>31</v>
       </c>
       <c r="B116">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C116" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D116" t="s">
-        <v>112</v>
-      </c>
-      <c r="E116" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
@@ -2772,16 +2863,13 @@
         <v>31</v>
       </c>
       <c r="B117">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C117" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D117" t="s">
-        <v>112</v>
-      </c>
-      <c r="E117" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
@@ -2789,16 +2877,13 @@
         <v>31</v>
       </c>
       <c r="B118">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C118" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D118" t="s">
-        <v>112</v>
-      </c>
-      <c r="E118" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
@@ -2806,16 +2891,16 @@
         <v>31</v>
       </c>
       <c r="B119">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C119" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D119" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E119" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
@@ -2823,16 +2908,16 @@
         <v>31</v>
       </c>
       <c r="B120">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C120" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D120" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E120" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
@@ -2840,186 +2925,177 @@
         <v>31</v>
       </c>
       <c r="B121">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C121" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D121" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E121" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B122">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C122" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D122" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
       <c r="E122" t="s">
-        <v>32</v>
+        <v>137</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B123">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C123" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D123" t="s">
-        <v>39</v>
+        <v>112</v>
       </c>
       <c r="E123" t="s">
-        <v>32</v>
+        <v>138</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B124">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C124" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D124" t="s">
-        <v>43</v>
+        <v>112</v>
       </c>
       <c r="E124" t="s">
-        <v>46</v>
+        <v>138</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B125">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C125" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D125" t="s">
-        <v>39</v>
+        <v>112</v>
       </c>
       <c r="E125" t="s">
-        <v>32</v>
+        <v>138</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B126">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C126" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D126" t="s">
-        <v>39</v>
+        <v>112</v>
       </c>
       <c r="E126" t="s">
-        <v>32</v>
+        <v>138</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B127">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C127" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D127" t="s">
-        <v>40</v>
+        <v>125</v>
       </c>
       <c r="E127" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B128">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C128" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D128" t="s">
-        <v>40</v>
+        <v>126</v>
       </c>
       <c r="E128" t="s">
-        <v>41</v>
+        <v>127</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>32</v>
       </c>
-      <c r="B129">
-        <v>2</v>
-      </c>
       <c r="C129" t="s">
-        <v>21</v>
+        <v>144</v>
       </c>
       <c r="D129" t="s">
-        <v>39</v>
+        <v>140</v>
       </c>
       <c r="E129" t="s">
-        <v>32</v>
+        <v>145</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>32</v>
       </c>
-      <c r="B130">
-        <v>3</v>
-      </c>
       <c r="C130" t="s">
-        <v>20</v>
+        <v>146</v>
       </c>
       <c r="D130" t="s">
-        <v>39</v>
+        <v>140</v>
       </c>
       <c r="E130" t="s">
-        <v>32</v>
+        <v>145</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>32</v>
       </c>
-      <c r="B131">
-        <v>3</v>
-      </c>
       <c r="C131" t="s">
-        <v>36</v>
+        <v>147</v>
       </c>
       <c r="D131" t="s">
-        <v>39</v>
+        <v>140</v>
       </c>
       <c r="E131" t="s">
-        <v>32</v>
+        <v>148</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -3027,16 +3103,16 @@
         <v>32</v>
       </c>
       <c r="B132">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C132" t="s">
-        <v>20</v>
+        <v>141</v>
       </c>
       <c r="D132" t="s">
-        <v>39</v>
+        <v>140</v>
       </c>
       <c r="E132" t="s">
-        <v>32</v>
+        <v>139</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -3044,237 +3120,237 @@
         <v>32</v>
       </c>
       <c r="B133">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C133" t="s">
-        <v>26</v>
+        <v>142</v>
       </c>
       <c r="D133" t="s">
-        <v>44</v>
+        <v>140</v>
       </c>
       <c r="E133" t="s">
-        <v>45</v>
+        <v>139</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B134">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C134" t="s">
-        <v>48</v>
+        <v>143</v>
       </c>
       <c r="D134" t="s">
-        <v>66</v>
+        <v>140</v>
       </c>
       <c r="E134" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B135">
         <v>1</v>
       </c>
       <c r="C135" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D135" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="E135" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B136">
         <v>1</v>
       </c>
       <c r="C136" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="D136" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="E136" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B137">
         <v>1</v>
       </c>
       <c r="C137" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D137" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="E137" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B138">
         <v>1</v>
       </c>
       <c r="C138" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="D138" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="E138" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B139">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C139" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D139" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="E139" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B140">
         <v>2</v>
       </c>
       <c r="C140" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="D140" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="E140" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B141">
         <v>2</v>
       </c>
       <c r="C141" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D141" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="E141" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B142">
         <v>2</v>
       </c>
       <c r="C142" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="D142" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="E142" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B143">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C143" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="D143" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="E143" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B144">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C144" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="D144" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="E144" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B145">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C145" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="D145" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="E145" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B146">
         <v>3</v>
       </c>
       <c r="C146" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="D146" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="E146" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
@@ -3282,16 +3358,16 @@
         <v>47</v>
       </c>
       <c r="B147">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C147" t="s">
-        <v>61</v>
+        <v>158</v>
       </c>
       <c r="D147" t="s">
-        <v>66</v>
+        <v>140</v>
       </c>
       <c r="E147" t="s">
-        <v>67</v>
+        <v>161</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
@@ -3299,16 +3375,16 @@
         <v>47</v>
       </c>
       <c r="B148">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C148" t="s">
-        <v>62</v>
+        <v>159</v>
       </c>
       <c r="D148" t="s">
-        <v>66</v>
+        <v>140</v>
       </c>
       <c r="E148" t="s">
-        <v>67</v>
+        <v>161</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
@@ -3319,370 +3395,361 @@
         <v>3</v>
       </c>
       <c r="C149" t="s">
-        <v>63</v>
+        <v>160</v>
       </c>
       <c r="D149" t="s">
-        <v>66</v>
+        <v>140</v>
       </c>
       <c r="E149" t="s">
-        <v>67</v>
+        <v>161</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>47</v>
       </c>
-      <c r="B150">
-        <v>3</v>
-      </c>
       <c r="C150" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="D150" t="s">
-        <v>66</v>
-      </c>
-      <c r="E150" t="s">
-        <v>68</v>
+        <v>140</v>
+      </c>
+      <c r="E150" s="4">
+        <v>44453</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>47</v>
       </c>
-      <c r="B151">
-        <v>3</v>
-      </c>
       <c r="C151" t="s">
-        <v>65</v>
+        <v>146</v>
       </c>
       <c r="D151" t="s">
-        <v>66</v>
-      </c>
-      <c r="E151" t="s">
-        <v>68</v>
+        <v>140</v>
+      </c>
+      <c r="E151" s="4">
+        <v>44453</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>69</v>
-      </c>
-      <c r="B152">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C152" t="s">
-        <v>70</v>
+        <v>147</v>
       </c>
       <c r="D152" t="s">
-        <v>78</v>
+        <v>140</v>
       </c>
       <c r="E152" t="s">
-        <v>42</v>
+        <v>148</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B153">
         <v>1</v>
       </c>
       <c r="C153" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="D153" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E153" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B154">
         <v>1</v>
       </c>
       <c r="C154" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="D154" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E154" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B155">
         <v>1</v>
       </c>
       <c r="C155" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="D155" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E155" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B156">
         <v>1</v>
       </c>
       <c r="C156" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D156" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E156" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B157">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C157" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="D157" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E157" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B158">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C158" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D158" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E158" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B159">
         <v>2</v>
       </c>
       <c r="C159" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="D159" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E159" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B160">
         <v>2</v>
       </c>
       <c r="C160" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D160" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E160" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B161">
         <v>2</v>
       </c>
       <c r="C161" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="D161" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E161" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B162">
         <v>2</v>
       </c>
       <c r="C162" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="D162" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E162" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B163">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C163" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="D163" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E163" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B164">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C164" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D164" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E164" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B165">
         <v>3</v>
       </c>
       <c r="C165" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="D165" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E165" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B166">
         <v>3</v>
       </c>
       <c r="C166" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="D166" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E166" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B167">
         <v>3</v>
       </c>
       <c r="C167" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="D167" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E167" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B168">
         <v>3</v>
       </c>
       <c r="C168" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="D168" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E168" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B169">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C169" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="D169" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E169" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B170">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C170" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="D170" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E170" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
@@ -3690,16 +3757,16 @@
         <v>69</v>
       </c>
       <c r="B171">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C171" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
       <c r="D171" t="s">
-        <v>78</v>
+        <v>140</v>
       </c>
       <c r="E171" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
@@ -3707,16 +3774,16 @@
         <v>69</v>
       </c>
       <c r="B172">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C172" t="s">
-        <v>88</v>
+        <v>155</v>
       </c>
       <c r="D172" t="s">
-        <v>78</v>
+        <v>140</v>
       </c>
       <c r="E172" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
@@ -3724,16 +3791,16 @@
         <v>69</v>
       </c>
       <c r="B173">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C173" t="s">
-        <v>89</v>
+        <v>156</v>
       </c>
       <c r="D173" t="s">
-        <v>78</v>
+        <v>140</v>
       </c>
       <c r="E173" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
@@ -3744,323 +3811,849 @@
         <v>4</v>
       </c>
       <c r="C174" t="s">
-        <v>90</v>
+        <v>157</v>
       </c>
       <c r="D174" t="s">
-        <v>78</v>
+        <v>140</v>
       </c>
       <c r="E174" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>92</v>
-      </c>
-      <c r="B175">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="C175" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
       <c r="D175" t="s">
-        <v>99</v>
-      </c>
-      <c r="E175" t="s">
-        <v>98</v>
+        <v>140</v>
+      </c>
+      <c r="E175" s="4">
+        <v>44453</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>92</v>
-      </c>
-      <c r="B176">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="C176" t="s">
-        <v>94</v>
+        <v>146</v>
       </c>
       <c r="D176" t="s">
-        <v>99</v>
-      </c>
-      <c r="E176" t="s">
-        <v>98</v>
+        <v>140</v>
+      </c>
+      <c r="E176" s="4">
+        <v>44453</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>92</v>
-      </c>
-      <c r="B177">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="C177" t="s">
-        <v>95</v>
+        <v>147</v>
       </c>
       <c r="D177" t="s">
-        <v>99</v>
+        <v>140</v>
       </c>
       <c r="E177" t="s">
-        <v>98</v>
+        <v>148</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B178">
         <v>1</v>
       </c>
       <c r="C178" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="D178" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="E178" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B179">
         <v>1</v>
       </c>
       <c r="C179" t="s">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="D179" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="E179" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B180">
         <v>1</v>
       </c>
       <c r="C180" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="D180" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="E180" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B181">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C181" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="D181" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="E181" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B182">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C182" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="D182" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="E182" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B183">
         <v>2</v>
       </c>
       <c r="C183" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="D183" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="E183" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B184">
         <v>2</v>
       </c>
       <c r="C184" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="D184" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="E184" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B185">
         <v>2</v>
       </c>
       <c r="C185" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="D185" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="E185" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B186">
         <v>2</v>
       </c>
       <c r="C186" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="D186" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="E186" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B187">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C187" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="D187" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="E187" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B188">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C188" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="D188" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="E188" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B189">
         <v>3</v>
       </c>
       <c r="C189" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="D189" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="E189" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B190">
         <v>3</v>
       </c>
       <c r="C190" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="D190" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="E190" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B191">
         <v>3</v>
       </c>
       <c r="C191" t="s">
-        <v>110</v>
+        <v>24</v>
       </c>
       <c r="D191" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="E191" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
+        <v>69</v>
+      </c>
+      <c r="B192">
+        <v>3</v>
+      </c>
+      <c r="C192" t="s">
+        <v>81</v>
+      </c>
+      <c r="D192" t="s">
+        <v>78</v>
+      </c>
+      <c r="E192" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>69</v>
+      </c>
+      <c r="B193">
+        <v>3</v>
+      </c>
+      <c r="C193" t="s">
+        <v>82</v>
+      </c>
+      <c r="D193" t="s">
+        <v>78</v>
+      </c>
+      <c r="E193" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>69</v>
+      </c>
+      <c r="B194">
+        <v>3</v>
+      </c>
+      <c r="C194" t="s">
+        <v>83</v>
+      </c>
+      <c r="D194" t="s">
+        <v>78</v>
+      </c>
+      <c r="E194" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>69</v>
+      </c>
+      <c r="B195">
+        <v>4</v>
+      </c>
+      <c r="C195" t="s">
+        <v>85</v>
+      </c>
+      <c r="D195" t="s">
+        <v>78</v>
+      </c>
+      <c r="E195" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>69</v>
+      </c>
+      <c r="B196">
+        <v>4</v>
+      </c>
+      <c r="C196" t="s">
+        <v>86</v>
+      </c>
+      <c r="D196" t="s">
+        <v>78</v>
+      </c>
+      <c r="E196" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>69</v>
+      </c>
+      <c r="B197">
+        <v>4</v>
+      </c>
+      <c r="C197" t="s">
+        <v>87</v>
+      </c>
+      <c r="D197" t="s">
+        <v>78</v>
+      </c>
+      <c r="E197" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>69</v>
+      </c>
+      <c r="B198">
+        <v>4</v>
+      </c>
+      <c r="C198" t="s">
+        <v>88</v>
+      </c>
+      <c r="D198" t="s">
+        <v>78</v>
+      </c>
+      <c r="E198" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>69</v>
+      </c>
+      <c r="B199">
+        <v>4</v>
+      </c>
+      <c r="C199" t="s">
+        <v>89</v>
+      </c>
+      <c r="D199" t="s">
+        <v>78</v>
+      </c>
+      <c r="E199" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>69</v>
+      </c>
+      <c r="B200">
+        <v>4</v>
+      </c>
+      <c r="C200" t="s">
+        <v>90</v>
+      </c>
+      <c r="D200" t="s">
+        <v>78</v>
+      </c>
+      <c r="E200" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
         <v>92</v>
       </c>
-      <c r="B192">
-        <v>3</v>
-      </c>
-      <c r="C192" t="s">
+      <c r="B201">
+        <v>1</v>
+      </c>
+      <c r="C201" t="s">
+        <v>162</v>
+      </c>
+      <c r="D201" t="s">
+        <v>140</v>
+      </c>
+      <c r="E201" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>92</v>
+      </c>
+      <c r="B202">
+        <v>2</v>
+      </c>
+      <c r="C202" t="s">
+        <v>164</v>
+      </c>
+      <c r="D202" t="s">
+        <v>140</v>
+      </c>
+      <c r="E202" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>92</v>
+      </c>
+      <c r="B203">
+        <v>3</v>
+      </c>
+      <c r="C203" t="s">
+        <v>163</v>
+      </c>
+      <c r="D203" t="s">
+        <v>140</v>
+      </c>
+      <c r="E203" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>92</v>
+      </c>
+      <c r="C204" t="s">
+        <v>144</v>
+      </c>
+      <c r="D204" t="s">
+        <v>140</v>
+      </c>
+      <c r="E204" s="4">
+        <v>44453</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>92</v>
+      </c>
+      <c r="C205" t="s">
+        <v>146</v>
+      </c>
+      <c r="D205" t="s">
+        <v>140</v>
+      </c>
+      <c r="E205" s="4">
+        <v>44453</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>92</v>
+      </c>
+      <c r="C206" t="s">
+        <v>147</v>
+      </c>
+      <c r="D206" t="s">
+        <v>140</v>
+      </c>
+      <c r="E206" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>92</v>
+      </c>
+      <c r="B207">
+        <v>1</v>
+      </c>
+      <c r="C207" t="s">
+        <v>93</v>
+      </c>
+      <c r="D207" t="s">
+        <v>99</v>
+      </c>
+      <c r="E207" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>92</v>
+      </c>
+      <c r="B208">
+        <v>1</v>
+      </c>
+      <c r="C208" t="s">
+        <v>94</v>
+      </c>
+      <c r="D208" t="s">
+        <v>99</v>
+      </c>
+      <c r="E208" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>92</v>
+      </c>
+      <c r="B209">
+        <v>1</v>
+      </c>
+      <c r="C209" t="s">
+        <v>95</v>
+      </c>
+      <c r="D209" t="s">
+        <v>99</v>
+      </c>
+      <c r="E209" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>92</v>
+      </c>
+      <c r="B210">
+        <v>1</v>
+      </c>
+      <c r="C210" t="s">
+        <v>9</v>
+      </c>
+      <c r="D210" t="s">
+        <v>99</v>
+      </c>
+      <c r="E210" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>92</v>
+      </c>
+      <c r="B211">
+        <v>1</v>
+      </c>
+      <c r="C211" t="s">
+        <v>96</v>
+      </c>
+      <c r="D211" t="s">
+        <v>99</v>
+      </c>
+      <c r="E211" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>92</v>
+      </c>
+      <c r="B212">
+        <v>1</v>
+      </c>
+      <c r="C212" t="s">
+        <v>97</v>
+      </c>
+      <c r="D212" t="s">
+        <v>99</v>
+      </c>
+      <c r="E212" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>92</v>
+      </c>
+      <c r="B213">
+        <v>2</v>
+      </c>
+      <c r="C213" t="s">
+        <v>101</v>
+      </c>
+      <c r="D213" t="s">
+        <v>100</v>
+      </c>
+      <c r="E213" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>92</v>
+      </c>
+      <c r="B214">
+        <v>2</v>
+      </c>
+      <c r="C214" t="s">
+        <v>102</v>
+      </c>
+      <c r="D214" t="s">
+        <v>100</v>
+      </c>
+      <c r="E214" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>92</v>
+      </c>
+      <c r="B215">
+        <v>2</v>
+      </c>
+      <c r="C215" t="s">
+        <v>103</v>
+      </c>
+      <c r="D215" t="s">
+        <v>100</v>
+      </c>
+      <c r="E215" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>92</v>
+      </c>
+      <c r="B216">
+        <v>2</v>
+      </c>
+      <c r="C216" t="s">
+        <v>104</v>
+      </c>
+      <c r="D216" t="s">
+        <v>100</v>
+      </c>
+      <c r="E216" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>92</v>
+      </c>
+      <c r="B217">
+        <v>2</v>
+      </c>
+      <c r="C217" t="s">
+        <v>16</v>
+      </c>
+      <c r="D217" t="s">
+        <v>100</v>
+      </c>
+      <c r="E217" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>92</v>
+      </c>
+      <c r="B218">
+        <v>2</v>
+      </c>
+      <c r="C218" t="s">
+        <v>105</v>
+      </c>
+      <c r="D218" t="s">
+        <v>100</v>
+      </c>
+      <c r="E218" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>92</v>
+      </c>
+      <c r="B219">
+        <v>3</v>
+      </c>
+      <c r="C219" t="s">
+        <v>106</v>
+      </c>
+      <c r="D219" t="s">
+        <v>111</v>
+      </c>
+      <c r="E219" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>92</v>
+      </c>
+      <c r="B220">
+        <v>3</v>
+      </c>
+      <c r="C220" t="s">
+        <v>107</v>
+      </c>
+      <c r="D220" t="s">
+        <v>111</v>
+      </c>
+      <c r="E220" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>92</v>
+      </c>
+      <c r="B221">
+        <v>3</v>
+      </c>
+      <c r="C221" t="s">
         <v>108</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D221" t="s">
         <v>111</v>
       </c>
-      <c r="E192" t="s">
+      <c r="E221" t="s">
         <v>98</v>
       </c>
     </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>92</v>
+      </c>
+      <c r="B222">
+        <v>3</v>
+      </c>
+      <c r="C222" t="s">
+        <v>109</v>
+      </c>
+      <c r="D222" t="s">
+        <v>111</v>
+      </c>
+      <c r="E222" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>92</v>
+      </c>
+      <c r="B223">
+        <v>3</v>
+      </c>
+      <c r="C223" t="s">
+        <v>110</v>
+      </c>
+      <c r="D223" t="s">
+        <v>111</v>
+      </c>
+      <c r="E223" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>92</v>
+      </c>
+      <c r="B224">
+        <v>3</v>
+      </c>
+      <c r="C224" t="s">
+        <v>108</v>
+      </c>
+      <c r="D224" t="s">
+        <v>111</v>
+      </c>
+      <c r="E224" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E49" xr:uid="{E18BD886-62ED-448C-B156-45B2284206D7}"/>
+  <autoFilter ref="A1:E56" xr:uid="{E18BD886-62ED-448C-B156-45B2284206D7}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4068,6 +4661,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -4079,15 +4681,6 @@
     <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4352,6 +4945,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA8A25A3-6E48-43DE-99F5-41171E7D2A04}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{555D9B9E-51F3-43B8-B2CA-3C8D9F5CDC6F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4359,14 +4960,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="42430076-c6fd-469b-b103-2493bbfbc263"/>
     <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA8A25A3-6E48-43DE-99F5-41171E7D2A04}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>